<commit_message>
update department model and seed
</commit_message>
<xml_diff>
--- a/helper/seed/Department.xlsx
+++ b/helper/seed/Department.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24020"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4336B3BB-35BA-492A-BB84-B6B2EB3F66FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C654C958-1130-48C2-83A8-613E557C87BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Mã đơn vị</t>
   </si>
@@ -34,7 +34,19 @@
     <t>Tên đơn vị</t>
   </si>
   <si>
-    <t>Có</t>
+    <t>Thuộc</t>
+  </si>
+  <si>
+    <t>PQLCL</t>
+  </si>
+  <si>
+    <t>Phòng quản lý chất lượng</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>Khoa Khoa học và Kỹ thuật máy tính</t>
   </si>
   <si>
     <t>MT-HTTT</t>
@@ -46,7 +58,7 @@
     <t>MT-KHMT</t>
   </si>
   <si>
-    <t xml:space="preserve">Khoa học máy tính </t>
+    <t>Khoa học máy tính</t>
   </si>
   <si>
     <t>MT-KTMT</t>
@@ -67,13 +79,52 @@
     <t>Khám phá tri thức</t>
   </si>
   <si>
-    <t>MT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Khoa Khoa học và Kỹ thuật máy tính </t>
-  </si>
-  <si>
-    <t>MT-HTTT,MT-KHMT,MT-KTMT</t>
+    <t>KHUD</t>
+  </si>
+  <si>
+    <t>Khoa Khoa học ứng dụng</t>
+  </si>
+  <si>
+    <t>KHUD-TUD</t>
+  </si>
+  <si>
+    <t>Toán ứng dụng</t>
+  </si>
+  <si>
+    <t>KHUD-CKT</t>
+  </si>
+  <si>
+    <t>Cơ Kỹ Thuật</t>
+  </si>
+  <si>
+    <t>KHUD-CHUD</t>
+  </si>
+  <si>
+    <t>Cơ học ứng dụng</t>
+  </si>
+  <si>
+    <t>KHUD-VLKT</t>
+  </si>
+  <si>
+    <t>Vật lý kỹ thuật</t>
+  </si>
+  <si>
+    <t>KHUD-VLUD</t>
+  </si>
+  <si>
+    <t>Vật lý ứng dụng</t>
+  </si>
+  <si>
+    <t>KHUD-VLDC</t>
+  </si>
+  <si>
+    <t>Vật lý đại cương</t>
+  </si>
+  <si>
+    <t>KHUD-LLCT</t>
+  </si>
+  <si>
+    <t>Lý luận chính trị</t>
   </si>
 </sst>
 </file>
@@ -109,10 +160,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,17 +488,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -453,13 +513,13 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0</v>
       </c>
     </row>
@@ -470,7 +530,7 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0</v>
       </c>
     </row>
@@ -481,8 +541,8 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -492,8 +552,8 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
-        <v>0</v>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -503,8 +563,8 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
-        <v>0</v>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -514,8 +574,107 @@
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 5/5 form + department
</commit_message>
<xml_diff>
--- a/helper/seed/Department.xlsx
+++ b/helper/seed/Department.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24102"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C654C958-1130-48C2-83A8-613E557C87BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44644D44-E86A-469B-B806-19BFB6F46F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -488,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -677,6 +677,17 @@
         <v>17</v>
       </c>
     </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>